<commit_message>
all matching layers losses fixed
</commit_message>
<xml_diff>
--- a/Reverse_anglesIn_60.xlsx
+++ b/Reverse_anglesIn_60.xlsx
@@ -440,7 +440,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>-0.5216745459112635</v>
+        <v>-0.5213247058072078</v>
       </c>
       <c r="B2" t="n">
         <v>59.99999999999999</v>
@@ -448,31 +448,31 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>-0.5096733457912509</v>
+        <v>-0.5093235056871952</v>
       </c>
       <c r="B3" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>-0.4976721456712409</v>
+        <v>-0.4973223055671844</v>
       </c>
       <c r="B4" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>-0.4856709455512273</v>
+        <v>-0.4853211054471715</v>
       </c>
       <c r="B5" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>-0.4736697454312156</v>
+        <v>-0.473319905327159</v>
       </c>
       <c r="B6" t="n">
         <v>59.99999999999999</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>-0.4616685453112032</v>
+        <v>-0.4613187052071479</v>
       </c>
       <c r="B7" t="n">
         <v>59.99999999999999</v>
@@ -488,15 +488,15 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>-0.4496673451911906</v>
+        <v>-0.4493175050871352</v>
       </c>
       <c r="B8" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>-0.4376661450711794</v>
+        <v>-0.4373163049671243</v>
       </c>
       <c r="B9" t="n">
         <v>59.99999999999999</v>
@@ -504,15 +504,15 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>-0.4256649449511669</v>
+        <v>-0.4253151048471118</v>
       </c>
       <c r="B10" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>-0.4136637448311555</v>
+        <v>-0.4133139047270988</v>
       </c>
       <c r="B11" t="n">
         <v>59.99999999999999</v>
@@ -520,15 +520,15 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>-0.4016625447111435</v>
+        <v>-0.4013127046070879</v>
       </c>
       <c r="B12" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>-0.3896613445911514</v>
+        <v>-0.3893115044870751</v>
       </c>
       <c r="B13" t="n">
         <v>59.99999999999999</v>
@@ -536,31 +536,31 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>-0.3776601444711178</v>
+        <v>-0.3773103043670641</v>
       </c>
       <c r="B14" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>-0.3656589443511068</v>
+        <v>-0.3653091042470514</v>
       </c>
       <c r="B15" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>-0.3536577442310964</v>
+        <v>-0.3533079041270387</v>
       </c>
       <c r="B16" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>-0.3416565441110834</v>
+        <v>-0.3413067040070281</v>
       </c>
       <c r="B17" t="n">
         <v>59.99999999999999</v>
@@ -568,23 +568,23 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>-0.3296553439910707</v>
+        <v>-0.3293055038870152</v>
       </c>
       <c r="B18" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>-0.31765414387106</v>
+        <v>-0.3173043037670042</v>
       </c>
       <c r="B19" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>-0.3056529437510471</v>
+        <v>-0.3053031036469915</v>
       </c>
       <c r="B20" t="n">
         <v>59.99999999999999</v>
@@ -592,23 +592,23 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>-0.2936517436310367</v>
+        <v>-0.2933019035269787</v>
       </c>
       <c r="B21" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>-0.2816505435110241</v>
+        <v>-0.2813007034069678</v>
       </c>
       <c r="B22" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>-0.2696493433910113</v>
+        <v>-0.2692995032869552</v>
       </c>
       <c r="B23" t="n">
         <v>59.99999999999999</v>
@@ -616,15 +616,15 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>-0.2576481432710014</v>
+        <v>-0.2572983031669421</v>
       </c>
       <c r="B24" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>-0.2456469431509883</v>
+        <v>-0.2452971030469315</v>
       </c>
       <c r="B25" t="n">
         <v>59.99999999999999</v>
@@ -632,15 +632,15 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>-0.2336457430309758</v>
+        <v>-0.2332959029269188</v>
       </c>
       <c r="B26" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>-0.2216445429109649</v>
+        <v>-0.2212947028069078</v>
       </c>
       <c r="B27" t="n">
         <v>59.99999999999999</v>
@@ -648,15 +648,15 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>-0.2096433427909529</v>
+        <v>-0.2092935026868951</v>
       </c>
       <c r="B28" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>-0.1976421426709416</v>
+        <v>-0.1972923025668823</v>
       </c>
       <c r="B29" t="n">
         <v>59.99999999999999</v>
@@ -664,15 +664,15 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>-0.185640942550929</v>
+        <v>-0.1852911024468715</v>
       </c>
       <c r="B30" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>-0.1736397424309164</v>
+        <v>-0.1732899023268587</v>
       </c>
       <c r="B31" t="n">
         <v>59.99999999999999</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>-0.161638542310906</v>
+        <v>-0.1612887022068477</v>
       </c>
       <c r="B32" t="n">
         <v>59.99999999999999</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>-0.1496373421908936</v>
+        <v>-0.1492875020868351</v>
       </c>
       <c r="B33" t="n">
         <v>59.99999999999999</v>
@@ -696,15 +696,15 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>-0.1376361420708831</v>
+        <v>-0.1372863019668224</v>
       </c>
       <c r="B34" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>-0.1256349419508704</v>
+        <v>-0.1252851018468114</v>
       </c>
       <c r="B35" t="n">
         <v>59.99999999999999</v>
@@ -712,39 +712,39 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>-0.1136337418308587</v>
+        <v>-0.1132839017267987</v>
       </c>
       <c r="B36" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>-0.101632541710848</v>
+        <v>-0.1012827016067876</v>
       </c>
       <c r="B37" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>-0.08963134159083529</v>
+        <v>-0.08928150148677495</v>
       </c>
       <c r="B38" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>-0.07763014147082543</v>
+        <v>-0.07728030136676217</v>
       </c>
       <c r="B39" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>-0.06562894135081271</v>
+        <v>-0.06527910124675149</v>
       </c>
       <c r="B40" t="n">
         <v>59.99999999999999</v>
@@ -752,39 +752,39 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>-0.05362774123080054</v>
+        <v>-0.05327790112673872</v>
       </c>
       <c r="B41" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>-0.04162654111079032</v>
+        <v>-0.0412767010067276</v>
       </c>
       <c r="B42" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>-0.02962534099077779</v>
+        <v>-0.02927550088671494</v>
       </c>
       <c r="B43" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>-0.01762414087076759</v>
+        <v>-0.01727430076670227</v>
       </c>
       <c r="B44" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>-0.005622940750755393</v>
+        <v>-0.005273100646691393</v>
       </c>
       <c r="B45" t="n">
         <v>59.99999999999999</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>0.006378259369257228</v>
+        <v>0.006728099473321326</v>
       </c>
       <c r="B46" t="n">
         <v>59.99999999999999</v>
@@ -800,31 +800,31 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>0.01837945948926704</v>
+        <v>0.01872929959333212</v>
       </c>
       <c r="B47" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>0.03038065960927907</v>
+        <v>0.03073049971334488</v>
       </c>
       <c r="B48" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>0.04238185972928952</v>
+        <v>0.04273169983335754</v>
       </c>
       <c r="B49" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>0.05438305984930228</v>
+        <v>0.05473289995336876</v>
       </c>
       <c r="B50" t="n">
         <v>59.99999999999999</v>
@@ -832,15 +832,15 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>0.06638425996931416</v>
+        <v>0.06673410007338143</v>
       </c>
       <c r="B51" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>0.07838546008932472</v>
+        <v>0.07873530019339216</v>
       </c>
       <c r="B52" t="n">
         <v>59.99999999999999</v>
@@ -848,15 +848,15 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>0.09038666020933674</v>
+        <v>0.09073650031340498</v>
       </c>
       <c r="B53" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>0.1023878603293474</v>
+        <v>0.1027377004334177</v>
       </c>
       <c r="B54" t="n">
         <v>59.99999999999999</v>
@@ -864,23 +864,23 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>0.1143890604493596</v>
+        <v>0.1147389005534286</v>
       </c>
       <c r="B55" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>0.1263902605693717</v>
+        <v>0.1267401006734413</v>
       </c>
       <c r="B56" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>0.1383914606893828</v>
+        <v>0.1387413007934522</v>
       </c>
       <c r="B57" t="n">
         <v>59.99999999999999</v>
@@ -888,15 +888,15 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>0.1503926608093951</v>
+        <v>0.150742500913465</v>
       </c>
       <c r="B58" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>0.162393860929406</v>
+        <v>0.1627437010334778</v>
       </c>
       <c r="B59" t="n">
         <v>59.99999999999999</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>0.1743950610494183</v>
+        <v>0.1747449011534887</v>
       </c>
       <c r="B60" t="n">
         <v>59.99999999999999</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>0.1863962611694308</v>
+        <v>0.1867461012735014</v>
       </c>
       <c r="B61" t="n">
         <v>59.99999999999999</v>
@@ -920,15 +920,15 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>0.1983974612894411</v>
+        <v>0.1987473013935121</v>
       </c>
       <c r="B62" t="n">
-        <v>60.00000000000004</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>0.2103986614094541</v>
+        <v>0.2107485015135249</v>
       </c>
       <c r="B63" t="n">
         <v>59.99999999999999</v>
@@ -936,15 +936,15 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>0.2223998615294651</v>
+        <v>0.2227497016335377</v>
       </c>
       <c r="B64" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>0.2344010616494781</v>
+        <v>0.2347509017535485</v>
       </c>
       <c r="B65" t="n">
         <v>59.99999999999999</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>0.2464022617695241</v>
+        <v>0.2467521018735614</v>
       </c>
       <c r="B66" t="n">
         <v>59.99999999999999</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>0.2584034618895207</v>
+        <v>0.2587533019935722</v>
       </c>
       <c r="B67" t="n">
         <v>59.99999999999999</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>0.2704046620095249</v>
+        <v>0.270754502113585</v>
       </c>
       <c r="B68" t="n">
         <v>59.99999999999999</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>0.2824058621295311</v>
+        <v>0.2827557022335979</v>
       </c>
       <c r="B69" t="n">
         <v>59.99999999999999</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>0.2944070622495409</v>
+        <v>0.2947569023536087</v>
       </c>
       <c r="B70" t="n">
         <v>59.99999999999999</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>0.306408262369552</v>
+        <v>0.3067581024736213</v>
       </c>
       <c r="B71" t="n">
         <v>59.99999999999999</v>
@@ -1000,15 +1000,15 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>0.3184094624895625</v>
+        <v>0.3187593025936323</v>
       </c>
       <c r="B72" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>0.3304106626095751</v>
+        <v>0.3307605027136449</v>
       </c>
       <c r="B73" t="n">
         <v>59.99999999999999</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>0.3424118627295863</v>
+        <v>0.3427617028336579</v>
       </c>
       <c r="B74" t="n">
         <v>59.99999999999999</v>
@@ -1024,15 +1024,15 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>0.3544130628495989</v>
+        <v>0.3547629029536686</v>
       </c>
       <c r="B75" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>0.3664142629696119</v>
+        <v>0.3667641030736813</v>
       </c>
       <c r="B76" t="n">
         <v>59.99999999999999</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>0.3784154630896235</v>
+        <v>0.3787653031936923</v>
       </c>
       <c r="B77" t="n">
         <v>59.99999999999999</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>0.3904166632096365</v>
+        <v>0.390766503313705</v>
       </c>
       <c r="B78" t="n">
         <v>59.99999999999999</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>0.4024178633296475</v>
+        <v>0.4027677034337177</v>
       </c>
       <c r="B79" t="n">
         <v>59.99999999999999</v>
@@ -1064,23 +1064,23 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>0.4144190634496606</v>
+        <v>0.4147689035537287</v>
       </c>
       <c r="B80" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>0.4264202635696737</v>
+        <v>0.4267701036737414</v>
       </c>
       <c r="B81" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>0.4384214636896847</v>
+        <v>0.4387713037937524</v>
       </c>
       <c r="B82" t="n">
         <v>59.99999999999999</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>0.4504226638096983</v>
+        <v>0.4507725039137651</v>
       </c>
       <c r="B83" t="n">
         <v>59.99999999999999</v>
@@ -1096,15 +1096,15 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>0.4624238639297171</v>
+        <v>0.4627737040337778</v>
       </c>
       <c r="B84" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>0.4744250640497223</v>
+        <v>0.474774904153789</v>
       </c>
       <c r="B85" t="n">
         <v>59.99999999999999</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>0.4864262641697362</v>
+        <v>0.4867761042738014</v>
       </c>
       <c r="B86" t="n">
         <v>59.99999999999999</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>0.4984274642897471</v>
+        <v>0.4987773043938125</v>
       </c>
       <c r="B87" t="n">
         <v>59.99999999999999</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>0.51042866440976</v>
+        <v>0.5107785045138252</v>
       </c>
       <c r="B88" t="n">
         <v>59.99999999999999</v>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>0.5224298645297716</v>
+        <v>0.5227797046338378</v>
       </c>
       <c r="B89" t="n">
-        <v>60.00000000000002</v>
+        <v>59.99999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>